<commit_message>
t/m kol 100 ok
</commit_message>
<xml_diff>
--- a/Utilities/python3/ToDO.xlsx
+++ b/Utilities/python3/ToDO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\cx1964ReposDWH\Utilities\python3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A586A8A7-4C2B-492D-8902-FB4CD7166AFA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB2F1A6-5216-4862-87B6-BD0CFF2AF620}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21720" yWindow="396" windowWidth="8352" windowHeight="13716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20220" yWindow="396" windowWidth="9852" windowHeight="13716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -784,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1048,124 +1048,124 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25">
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26">
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="29" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="30" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30">
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="31" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31">
+      <c r="B31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B32" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32">
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1">
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="33" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33">
+      <c r="B33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1">
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="34" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34">
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
t/m col 82 ok
</commit_message>
<xml_diff>
--- a/Utilities/python3/ToDO.xlsx
+++ b/Utilities/python3/ToDO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\cx1964ReposDWH\Utilities\python3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020E04DC-BB4C-43D4-A413-185956EFA4FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08DF233F-C3DD-4E0F-8334-075DFD713623}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12516" yWindow="624" windowWidth="13224" windowHeight="13716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17412" yWindow="672" windowWidth="13224" windowHeight="13716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="141">
   <si>
     <t>column_name</t>
   </si>
@@ -785,7 +785,7 @@
   <dimension ref="A1:M133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89:XFD89"/>
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2027,69 +2027,69 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row r="83" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B83" t="s">
-        <v>12</v>
-      </c>
-      <c r="C83">
+      <c r="B83" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C83" s="1">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="84" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B84" t="s">
-        <v>12</v>
-      </c>
-      <c r="C84">
+      <c r="B84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="85" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B85" t="s">
-        <v>4</v>
-      </c>
-      <c r="C85">
+      <c r="B85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" s="1">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row r="86" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B86" t="s">
-        <v>12</v>
-      </c>
-      <c r="C86">
+      <c r="B86" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" s="1">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="87" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B87" t="s">
-        <v>4</v>
-      </c>
-      <c r="C87">
+      <c r="B87" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" s="1">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+    <row r="88" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B88" t="s">
-        <v>12</v>
-      </c>
-      <c r="C88">
+      <c r="B88" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C88" s="1">
         <v>87</v>
       </c>
     </row>

</xml_diff>

<commit_message>
is mogelijk met datum veld
</commit_message>
<xml_diff>
--- a/Utilities/python3/ToDO.xlsx
+++ b/Utilities/python3/ToDO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\cx1964ReposDWH\Utilities\python3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C81756D-0CDD-4015-9E5A-5AD55ECFDC38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55336C5-E429-49CA-90B1-A0789A70524C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17412" yWindow="672" windowWidth="13224" windowHeight="13716" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17328" yWindow="252" windowWidth="13224" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -454,10 +454,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -470,8 +477,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,6 +504,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -503,12 +523,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -791,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="F116" sqref="F116"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1660,7 +1683,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -1671,7 +1694,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -1682,7 +1705,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>90</v>
       </c>
@@ -1693,7 +1716,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>89</v>
       </c>
@@ -1704,7 +1727,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -1715,7 +1738,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>87</v>
       </c>
@@ -1726,7 +1749,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>86</v>
       </c>
@@ -1737,7 +1760,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -1748,7 +1771,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>84</v>
       </c>
@@ -1759,7 +1782,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>83</v>
       </c>
@@ -1770,7 +1793,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>82</v>
       </c>
@@ -1781,7 +1804,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>81</v>
       </c>
@@ -1792,7 +1815,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>80</v>
       </c>
@@ -1803,7 +1826,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -1814,7 +1837,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -1825,16 +1848,20 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="64" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="1">
         <v>63</v>
       </c>
+      <c r="D64" s="6"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
@@ -1980,7 +2007,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+      <c r="A78" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B78" t="s">

</xml_diff>

<commit_message>
tussen versie 20200407 9:34 werkt
</commit_message>
<xml_diff>
--- a/Utilities/python3/ToDO.xlsx
+++ b/Utilities/python3/ToDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\cx1964ReposDWH\Utilities\python3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4153F50D-067E-47B2-AB73-A8A57C75EE40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3F9CAC-BCC3-47A7-B51D-9C970D571F91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22044" yWindow="456" windowWidth="8688" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,17 +454,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -529,16 +522,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -821,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1865,19 +1857,19 @@
       <c r="C64" s="1">
         <v>63</v>
       </c>
-      <c r="D64" s="6"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-    </row>
-    <row r="65" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="8" t="s">
+      <c r="D64" s="5"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="8">
+      <c r="C65" s="7">
         <v>64</v>
       </c>
     </row>
@@ -2013,14 +2005,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="5" t="s">
+    <row r="78" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="1">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
werkende tussen versie 20200407 9:43
</commit_message>
<xml_diff>
--- a/Utilities/python3/ToDO.xlsx
+++ b/Utilities/python3/ToDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\cx1964ReposDWH\Utilities\python3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3F9CAC-BCC3-47A7-B51D-9C970D571F91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520E86D6-C1B3-446F-940E-343B48F9F953}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22044" yWindow="456" windowWidth="8688" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -814,7 +814,7 @@
   <dimension ref="A1:M133"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+      <selection activeCell="A75" sqref="A75:XFD75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1972,36 +1972,36 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="75" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="76" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B76" t="s">
-        <v>4</v>
-      </c>
-      <c r="C76">
+      <c r="B76" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="77" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C77">
+      <c r="B77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="1">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
werkt tussenwaarde 20200407 10:02
</commit_message>
<xml_diff>
--- a/Utilities/python3/ToDO.xlsx
+++ b/Utilities/python3/ToDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\cx1964ReposDWH\Utilities\python3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520E86D6-C1B3-446F-940E-343B48F9F953}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1942A2AB-7128-4EC5-B1C3-3ABD02F3B211}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22044" yWindow="456" windowWidth="8688" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,7 +454,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,19 +472,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,12 +496,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -522,15 +509,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -813,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:XFD75"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1627,223 +1612,223 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="44" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B44" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44">
+      <c r="B44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="45" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45">
+      <c r="B45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row r="46" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B46" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46">
+      <c r="B46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="47" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B47" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47">
+      <c r="B47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="48" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B48" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48">
+      <c r="B48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="49" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B49" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49">
+      <c r="B49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="50" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B50" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50">
+      <c r="B50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="51" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B51" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51">
+      <c r="B51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="52" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B52" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52">
+      <c r="B52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="53" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B53" t="s">
-        <v>12</v>
-      </c>
-      <c r="C53">
+      <c r="B53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="54" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54">
+      <c r="B54" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="55" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55">
+      <c r="B55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="1">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="56" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B56" t="s">
-        <v>12</v>
-      </c>
-      <c r="C56">
+      <c r="B56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="1">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="57" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B57" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57">
+      <c r="B57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="58" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B58" t="s">
-        <v>12</v>
-      </c>
-      <c r="C58">
+      <c r="B58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" s="1">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="59" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B59" t="s">
-        <v>12</v>
-      </c>
-      <c r="C59">
+      <c r="B59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="1">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="60" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B60" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60">
+      <c r="B60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="1">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="61" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B61" t="s">
-        <v>12</v>
-      </c>
-      <c r="C61">
+      <c r="B61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="62" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B62" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62">
+      <c r="B62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="1">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="63" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B63" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63">
+      <c r="B63" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C63" s="1">
         <v>62</v>
       </c>
     </row>
@@ -1858,18 +1843,18 @@
         <v>63</v>
       </c>
       <c r="D64" s="5"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="6"/>
-      <c r="G64" s="6"/>
-    </row>
-    <row r="65" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="7" t="s">
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+    </row>
+    <row r="65" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="5">
         <v>64</v>
       </c>
     </row>
@@ -1884,91 +1869,91 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="67" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B67" t="s">
-        <v>4</v>
-      </c>
-      <c r="C67">
+      <c r="B67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="1">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="68" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B68" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68">
+      <c r="B68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="69" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="1">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="70" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B70" t="s">
-        <v>12</v>
-      </c>
-      <c r="C70">
+      <c r="B70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="71" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B71" t="s">
-        <v>4</v>
-      </c>
-      <c r="C71">
+      <c r="B71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="72" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B72" t="s">
-        <v>4</v>
-      </c>
-      <c r="C72">
+      <c r="B72" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row r="73" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B73" t="s">
-        <v>4</v>
-      </c>
-      <c r="C73">
+      <c r="B73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row r="74" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B74" t="s">
-        <v>4</v>
-      </c>
-      <c r="C74">
+      <c r="B74" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="1">
         <v>73</v>
       </c>
     </row>
@@ -2006,7 +1991,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B78" s="1" t="s">

</xml_diff>

<commit_message>
Final werkende testversie elm3
</commit_message>
<xml_diff>
--- a/Utilities/python3/ToDO.xlsx
+++ b/Utilities/python3/ToDO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\cx1964ReposDWH\Utilities\python3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1942A2AB-7128-4EC5-B1C3-3ABD02F3B211}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC02C549-A000-494C-8083-CAA65ED7DC9A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22044" yWindow="456" windowWidth="8688" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -796,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M133"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,7 +809,7 @@
     <col min="3" max="3" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -820,799 +820,469 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-    </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4"/>
-    </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-    </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1">
         <v>5</v>
       </c>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-    </row>
-    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    </row>
+    <row r="7" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>6</v>
       </c>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    </row>
+    <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
         <v>7</v>
       </c>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8"/>
-    </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    </row>
+    <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1">
         <v>8</v>
       </c>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-    </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    </row>
+    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
         <v>9</v>
       </c>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
-    </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    </row>
+    <row r="11" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
         <v>10</v>
       </c>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    </row>
+    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1">
         <v>11</v>
       </c>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-    </row>
-    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    </row>
+    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-    </row>
-    <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1">
         <v>13</v>
       </c>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-    </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    </row>
+    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>14</v>
       </c>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-    </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    </row>
+    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
         <v>15</v>
       </c>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-    </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    </row>
+    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1">
         <v>16</v>
       </c>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
-      <c r="K17"/>
-      <c r="L17"/>
-      <c r="M17"/>
-    </row>
-    <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    </row>
+    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1">
         <v>17</v>
       </c>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-      <c r="I18"/>
-      <c r="J18"/>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-    </row>
-    <row r="19" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    </row>
+    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1">
         <v>18</v>
       </c>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-    </row>
-    <row r="20" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    </row>
+    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>19</v>
       </c>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-    </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    </row>
+    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21">
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1">
         <v>20</v>
       </c>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
-      <c r="M21"/>
-    </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    </row>
+    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1">
         <v>21</v>
       </c>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-    </row>
-    <row r="23" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    </row>
+    <row r="23" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23">
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
         <v>22</v>
       </c>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-      <c r="I23"/>
-      <c r="J23"/>
-      <c r="K23"/>
-      <c r="L23"/>
-      <c r="M23"/>
-    </row>
-    <row r="24" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    </row>
+    <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="1">
         <v>23</v>
       </c>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-      <c r="I24"/>
-      <c r="J24"/>
-      <c r="K24"/>
-      <c r="L24"/>
-      <c r="M24"/>
-    </row>
-    <row r="25" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    </row>
+    <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25">
+      <c r="B25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1">
         <v>24</v>
       </c>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25"/>
-      <c r="K25"/>
-      <c r="L25"/>
-      <c r="M25"/>
-    </row>
-    <row r="26" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    </row>
+    <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26">
+      <c r="B26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1">
         <v>25</v>
       </c>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
-      <c r="I26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-    </row>
-    <row r="27" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    </row>
+    <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1">
         <v>26</v>
       </c>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27"/>
-      <c r="I27"/>
-      <c r="J27"/>
-      <c r="K27"/>
-      <c r="L27"/>
-      <c r="M27"/>
-    </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    </row>
+    <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="1">
         <v>27</v>
       </c>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
-      <c r="J28"/>
-      <c r="K28"/>
-      <c r="L28"/>
-      <c r="M28"/>
-    </row>
-    <row r="29" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    </row>
+    <row r="29" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="1">
         <v>28</v>
       </c>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29"/>
-    </row>
-    <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    </row>
+    <row r="30" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <v>29</v>
       </c>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-      <c r="I30"/>
-      <c r="J30"/>
-      <c r="K30"/>
-      <c r="L30"/>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    </row>
+    <row r="31" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31">
+      <c r="B31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1">
         <v>30</v>
       </c>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-    </row>
-    <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    </row>
+    <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32">
+      <c r="B32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="1">
         <v>31</v>
       </c>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
-      <c r="I32"/>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32"/>
-    </row>
-    <row r="33" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    </row>
+    <row r="33" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33">
+      <c r="B33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1">
         <v>32</v>
       </c>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
-      <c r="M33"/>
-    </row>
-    <row r="34" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    </row>
+    <row r="34" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34">
+      <c r="B34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="1">
         <v>33</v>
       </c>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-      <c r="I34"/>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    </row>
+    <row r="35" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35">
+      <c r="B35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="36" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36">
+      <c r="B36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row r="37" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37">
+      <c r="B37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="1">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="38" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C38">
+      <c r="B38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="39" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B39" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39">
+      <c r="B39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40">
+      <c r="B40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="41" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41">
+      <c r="B41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="42" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42">
+      <c r="B42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="43" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B43" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43">
+      <c r="B43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>97</v>
       </c>
@@ -1623,7 +1293,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>96</v>
       </c>
@@ -1634,7 +1304,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>95</v>
       </c>
@@ -1645,7 +1315,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>94</v>
       </c>
@@ -1656,7 +1326,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>93</v>
       </c>

</xml_diff>